<commit_message>
Décalage de la tâche de Jaime du 14/11/2014 au 16/11/2014
</commit_message>
<xml_diff>
--- a/Tache.xlsx
+++ b/Tache.xlsx
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +591,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="9">
-        <v>41955</v>
+        <v>41956</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>8</v>
@@ -606,7 +606,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="9">
-        <v>41956</v>
+        <v>41957</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>8</v>
@@ -621,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="9">
-        <v>41957</v>
+        <v>41959</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>

</xml_diff>